<commit_message>
SchoolDepartment.feature SchoolDepartments.java     ->>Delete Added And This UserStory is Done
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
+++ b/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Add New School Department</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>Edit School Department</t>
+  </si>
+  <si>
+    <t>Add Position Categories</t>
+  </si>
+  <si>
+    <t>Edit Position Categories</t>
+  </si>
+  <si>
+    <t>Delete Position Categories</t>
+  </si>
+  <si>
+    <t>Delete The School Department</t>
   </si>
 </sst>
 </file>
@@ -381,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -403,6 +415,54 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CampusBankAccounts.xlsx BankAccounts.feature BankAccountsSteps.java ADDED any Locators added
BankAccounts.feature is DONE
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
+++ b/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senol\IdeaProjects\mersys.io\src\test\java\ApachePOI\"/>
     </mc:Choice>
@@ -20,11 +20,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+  <si>
+    <t>Add New Bank Accounts</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>Edit The Bank Accounts</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>Delete The Bank Accounts</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,12 +390,79 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CampusBankAccounts.xlsx deleted CampusBankAccounts.xlsx added Nationalities.feature added DialogPage.java locator added LeftBar.java Locator added NationalitiesSteps.java added
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
+++ b/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="7">
   <si>
     <t>Add New Bank Accounts</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Delete The Bank Accounts</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -390,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,6 +465,83 @@
         <v>2</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
HumanResourcesAttestation.feature -> added HumanResourcesAttestationSteps.java -> added DialogPage.java -> any Locators added LeftBar.java -> any Locators added
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
+++ b/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="15">
   <si>
     <t>Add New Bank Accounts</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>User Delete the School Locations</t>
+  </si>
+  <si>
+    <t>The Admin Add Edit and Delete Attestations under Human Resources</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -904,6 +907,512 @@
         <v>2</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>14</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>14</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>14</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>14</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>14</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>14</v>
+      </c>
+      <c r="B69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>14</v>
+      </c>
+      <c r="B70" t="s">
+        <v>4</v>
+      </c>
+      <c r="C70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>14</v>
+      </c>
+      <c r="B76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>14</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>14</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>14</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>14</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>14</v>
+      </c>
+      <c r="B85" t="s">
+        <v>4</v>
+      </c>
+      <c r="C85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>14</v>
+      </c>
+      <c r="B86" t="s">
+        <v>4</v>
+      </c>
+      <c r="C86" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>14</v>
+      </c>
+      <c r="B87" t="s">
+        <v>4</v>
+      </c>
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>14</v>
+      </c>
+      <c r="B88" t="s">
+        <v>4</v>
+      </c>
+      <c r="C88" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>14</v>
+      </c>
+      <c r="B89" t="s">
+        <v>4</v>
+      </c>
+      <c r="C89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>14</v>
+      </c>
+      <c r="B90" t="s">
+        <v>4</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
PositionsSteps_Tuba positive and negative test created
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
+++ b/src/test/java/ApachePOI/SenaryoSonuclari.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="20">
   <si>
     <t>Add New Bank Accounts</t>
   </si>
@@ -71,6 +71,15 @@
   </si>
   <si>
     <t>Edit</t>
+  </si>
+  <si>
+    <t>Login with valid username and password</t>
+  </si>
+  <si>
+    <t>Adding New Positions to the Admin Panel</t>
+  </si>
+  <si>
+    <t>UNDEFINED</t>
   </si>
 </sst>
 </file>
@@ -423,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1749,6 +1758,325 @@
         <v>2</v>
       </c>
     </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>17</v>
+      </c>
+      <c r="B121" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>17</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>0</v>
+      </c>
+      <c r="B123" t="s">
+        <v>1</v>
+      </c>
+      <c r="C123" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" t="s">
+        <v>1</v>
+      </c>
+      <c r="C125" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>18</v>
+      </c>
+      <c r="B126" t="s">
+        <v>1</v>
+      </c>
+      <c r="C126" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>18</v>
+      </c>
+      <c r="B127" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>18</v>
+      </c>
+      <c r="B128" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>18</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>18</v>
+      </c>
+      <c r="B130" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>18</v>
+      </c>
+      <c r="B131" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>18</v>
+      </c>
+      <c r="B132" t="s">
+        <v>1</v>
+      </c>
+      <c r="C132" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>18</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>18</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>18</v>
+      </c>
+      <c r="B135" t="s">
+        <v>1</v>
+      </c>
+      <c r="C135" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>18</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>18</v>
+      </c>
+      <c r="B137" t="s">
+        <v>1</v>
+      </c>
+      <c r="C137" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>18</v>
+      </c>
+      <c r="B138" t="s">
+        <v>1</v>
+      </c>
+      <c r="C138" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>18</v>
+      </c>
+      <c r="B139" t="s">
+        <v>1</v>
+      </c>
+      <c r="C139" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>18</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>18</v>
+      </c>
+      <c r="B141" t="s">
+        <v>19</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>18</v>
+      </c>
+      <c r="B142" t="s">
+        <v>19</v>
+      </c>
+      <c r="C142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>18</v>
+      </c>
+      <c r="B143" t="s">
+        <v>19</v>
+      </c>
+      <c r="C143" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>18</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>18</v>
+      </c>
+      <c r="B145" t="s">
+        <v>4</v>
+      </c>
+      <c r="C145" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>18</v>
+      </c>
+      <c r="B146" t="s">
+        <v>4</v>
+      </c>
+      <c r="C146" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>18</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>18</v>
+      </c>
+      <c r="B148" t="s">
+        <v>1</v>
+      </c>
+      <c r="C148" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>18</v>
+      </c>
+      <c r="B149" t="s">
+        <v>4</v>
+      </c>
+      <c r="C149" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>